<commit_message>
Inicializando a Interface do conversor
Iniciado o conversor de temperatura (html e javascript) e atualizado do
Daily Scrum
</commit_message>
<xml_diff>
--- a/Daily Scrum.xlsx
+++ b/Daily Scrum.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Daily Scrum</t>
   </si>
@@ -97,6 +97,33 @@
   </si>
   <si>
     <t>Corrigir os erros do dia anterior e concluir Story</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Inciando a interface o conversor de temperatura</t>
+  </si>
+  <si>
+    <t>Foi inserido a interface inicial do conversor de temperatura</t>
+  </si>
+  <si>
+    <t>Iniciando o javascript para a interface inicial do conversor</t>
+  </si>
+  <si>
+    <t>Alguns itens ainda não estam funcionais (problemas)</t>
+  </si>
+  <si>
+    <t>Implementado javascript no conversor de temperatura</t>
+  </si>
+  <si>
+    <t>Finalizando o javascript para interface inicial do conversor</t>
+  </si>
+  <si>
+    <t>Iniciando a interface final do conversor de temperatura</t>
+  </si>
+  <si>
+    <t>Iniciando o javascript para a interface final do conversor</t>
   </si>
 </sst>
 </file>
@@ -298,9 +325,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,9 +342,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,6 +351,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +652,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,16 +679,16 @@
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2"/>
@@ -676,22 +701,22 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>41822</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="2"/>
@@ -717,7 +742,7 @@
       <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -726,7 +751,7 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="16">
+      <c r="A5" s="18">
         <v>41824</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -741,7 +766,7 @@
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -750,7 +775,7 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
@@ -759,7 +784,7 @@
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -768,7 +793,7 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="16">
+      <c r="A7" s="18">
         <v>41825</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -777,13 +802,13 @@
       <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -792,7 +817,7 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="16"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>13</v>
@@ -801,7 +826,7 @@
       <c r="E8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -810,22 +835,22 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>41826</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -834,20 +859,20 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>41827</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="2"/>
@@ -858,22 +883,22 @@
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>41828</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -882,20 +907,20 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>41829</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -904,14 +929,20 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>41830</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="18"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -920,14 +951,20 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>41831</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="18"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -936,14 +973,18 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>41832</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="18"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="16"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -952,14 +993,22 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>41833</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="18"/>
+      <c r="B16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="16"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -968,14 +1017,20 @@
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>41834</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="17"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -985,10 +1040,12 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -999,9 +1056,11 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>

</xml_diff>

<commit_message>
Corrigindo os defeitos no Histórico e no Conversor
</commit_message>
<xml_diff>
--- a/Daily Scrum.xlsx
+++ b/Daily Scrum.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>Daily Scrum</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Iniciando o javascript para a interface final do conversor</t>
+  </si>
+  <si>
+    <t>Atuar no defeito do conversor e do histórico</t>
+  </si>
+  <si>
+    <t>Concluido a correção nos defeitos</t>
   </si>
 </sst>
 </file>
@@ -173,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -304,11 +310,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -342,6 +381,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -354,7 +394,15 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +700,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -716,7 +764,7 @@
       <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="2"/>
@@ -742,7 +790,7 @@
       <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -751,7 +799,7 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="18">
+      <c r="A5" s="19">
         <v>41824</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -766,7 +814,7 @@
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -775,7 +823,7 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
@@ -784,7 +832,7 @@
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -793,7 +841,7 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="18">
+      <c r="A7" s="19">
         <v>41825</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -808,7 +856,7 @@
       <c r="E7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -817,7 +865,7 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>13</v>
@@ -826,7 +874,7 @@
       <c r="E8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -850,7 +898,7 @@
       <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="18"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -872,7 +920,7 @@
       <c r="E10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="2"/>
@@ -898,7 +946,7 @@
       <c r="E11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -920,7 +968,7 @@
       <c r="E12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -942,7 +990,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="16"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -964,7 +1012,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="16"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -984,7 +1032,7 @@
       <c r="E15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1008,7 +1056,7 @@
       <c r="E16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1017,7 +1065,7 @@
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="9">
+      <c r="A17" s="20">
         <v>41834</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1030,7 +1078,7 @@
       <c r="E17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1039,13 +1087,13 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="19"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="15"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1055,12 +1103,12 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1071,11 +1119,17 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="2"/>
+      <c r="A20" s="5">
+        <v>41835</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1085,11 +1139,17 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="2"/>
+      <c r="A21" s="5">
+        <v>41836</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1265,11 +1325,12 @@
       <c r="I35" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="F10:F17"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="F3:F9"/>
+    <mergeCell ref="A17:A19"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizando o Daily Scrum
versão final da calculadora
</commit_message>
<xml_diff>
--- a/Daily Scrum.xlsx
+++ b/Daily Scrum.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="24855" windowHeight="12015"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Daily Scrum</t>
   </si>
@@ -130,13 +130,43 @@
   </si>
   <si>
     <t>Concluido a correção nos defeitos</t>
+  </si>
+  <si>
+    <t>Verifiquei as mudanças efetuadas, planejei melhorias e fiz um esboço para codificar</t>
+  </si>
+  <si>
+    <t>Klébson</t>
+  </si>
+  <si>
+    <t>Codifiquei as mudanças previstas (melhorias)</t>
+  </si>
+  <si>
+    <t>sim. Resultado insatisfatório (fugindo do esboço)</t>
+  </si>
+  <si>
+    <t>Simplifiquei os códigos, corrigir bugs e modifiquei estrutura</t>
+  </si>
+  <si>
+    <t>Ajustar o código para atender as especificações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">não. </t>
+  </si>
+  <si>
+    <t>00-07-2014</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Ronaldo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,6 +412,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -400,8 +433,8 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,6 +442,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -487,6 +525,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -521,6 +560,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -696,14 +736,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -712,7 +752,7 @@
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -726,7 +766,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -748,7 +788,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>41822</v>
       </c>
@@ -764,7 +804,7 @@
       <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="2"/>
@@ -774,7 +814,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>41823</v>
       </c>
@@ -790,7 +830,7 @@
       <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -798,8 +838,8 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="19">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
         <v>41824</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -814,7 +854,7 @@
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -822,8 +862,8 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
@@ -832,7 +872,7 @@
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -840,8 +880,8 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="19">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
         <v>41825</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -856,7 +896,7 @@
       <c r="E7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -864,8 +904,8 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="19"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>13</v>
@@ -874,7 +914,7 @@
       <c r="E8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -882,7 +922,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>41826</v>
       </c>
@@ -898,7 +938,7 @@
       <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -906,7 +946,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>41827</v>
       </c>
@@ -920,7 +960,7 @@
       <c r="E10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="17" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="2"/>
@@ -930,7 +970,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>41828</v>
       </c>
@@ -946,7 +986,7 @@
       <c r="E11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -954,7 +994,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>41829</v>
       </c>
@@ -968,7 +1008,7 @@
       <c r="E12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="17"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -976,7 +1016,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>41830</v>
       </c>
@@ -990,7 +1030,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="17"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -998,7 +1038,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>41831</v>
       </c>
@@ -1012,7 +1052,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="17"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1020,7 +1060,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>41832</v>
       </c>
@@ -1032,7 +1072,7 @@
       <c r="E15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1040,7 +1080,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>41833</v>
       </c>
@@ -1056,7 +1096,7 @@
       <c r="E16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="17"/>
+      <c r="F16" s="18"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1064,8 +1104,8 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="20">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
         <v>41834</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1086,15 +1126,17 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="21"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="23" t="s">
+        <v>20</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1102,15 +1144,15 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1118,7 +1160,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>41835</v>
       </c>
@@ -1130,7 +1172,7 @@
       <c r="E20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1138,7 +1180,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>41836</v>
       </c>
@@ -1150,7 +1192,7 @@
       <c r="E21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1158,13 +1200,23 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>41837</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="23"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1172,13 +1224,23 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>41837</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="23"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1186,13 +1248,17 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="23"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1200,13 +1266,17 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="23"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1214,40 +1284,61 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="23"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="23"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="23"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1258,7 +1349,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1269,7 +1360,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1280,7 +1371,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1291,7 +1382,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1302,7 +1393,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1313,7 +1404,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1325,12 +1416,13 @@
       <c r="I35" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="F10:F17"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="F3:F9"/>
     <mergeCell ref="A17:A19"/>
+    <mergeCell ref="F18:F28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1338,24 +1430,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Teste realizado e Atuando nas Correções
</commit_message>
<xml_diff>
--- a/Daily Scrum.xlsx
+++ b/Daily Scrum.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="20730" windowHeight="11760"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>Daily Scrum</t>
   </si>
@@ -153,20 +153,20 @@
     <t xml:space="preserve">não. </t>
   </si>
   <si>
-    <t>00-07-2014</t>
-  </si>
-  <si>
-    <t>Anderson</t>
-  </si>
-  <si>
-    <t>Ronaldo</t>
+    <t>Realizado ajustes no "CE" da calculadora</t>
+  </si>
+  <si>
+    <t>Implementado uma nova interface e testes</t>
+  </si>
+  <si>
+    <t>Problemas no "CE" para número</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,10 +421,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -525,7 +525,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -560,7 +559,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -736,23 +734,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -766,7 +764,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -788,7 +786,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="10">
         <v>41822</v>
       </c>
@@ -814,7 +812,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="5">
         <v>41823</v>
       </c>
@@ -838,8 +836,8 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+    <row r="5" spans="1:12">
+      <c r="A5" s="19">
         <v>41824</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -862,8 +860,8 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:12">
+      <c r="A6" s="19"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>13</v>
@@ -880,8 +878,8 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+    <row r="7" spans="1:12">
+      <c r="A7" s="19">
         <v>41825</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -904,8 +902,8 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+    <row r="8" spans="1:12">
+      <c r="A8" s="19"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>13</v>
@@ -922,7 +920,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1">
       <c r="A9" s="9">
         <v>41826</v>
       </c>
@@ -938,7 +936,7 @@
       <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -946,7 +944,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="9">
         <v>41827</v>
       </c>
@@ -970,7 +968,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="9">
         <v>41828</v>
       </c>
@@ -994,7 +992,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="9">
         <v>41829</v>
       </c>
@@ -1016,7 +1014,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="9">
         <v>41830</v>
       </c>
@@ -1038,7 +1036,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="9">
         <v>41831</v>
       </c>
@@ -1060,7 +1058,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="9">
         <v>41832</v>
       </c>
@@ -1080,7 +1078,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="9">
         <v>41833</v>
       </c>
@@ -1104,7 +1102,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="21">
         <v>41834</v>
       </c>
@@ -1126,7 +1124,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="22"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
@@ -1144,7 +1142,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="22"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16" t="s">
@@ -1160,7 +1158,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="5">
         <v>41835</v>
       </c>
@@ -1180,7 +1178,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="5">
         <v>41836</v>
       </c>
@@ -1200,7 +1198,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="5">
         <v>41837</v>
       </c>
@@ -1224,7 +1222,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="5">
         <v>41837</v>
       </c>
@@ -1248,16 +1246,14 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>45</v>
+    <row r="24" spans="1:12">
+      <c r="A24" s="5">
+        <v>41838</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="E24" s="15"/>
       <c r="F24" s="23"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1266,15 +1262,19 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>45</v>
+    <row r="25" spans="1:12">
+      <c r="A25" s="5">
+        <v>41839</v>
       </c>
       <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="E25" s="15" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25" s="2"/>
@@ -1284,15 +1284,19 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:12">
+      <c r="A26" s="5">
+        <v>41840</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="15" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="2"/>
@@ -1302,16 +1306,14 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>45</v>
+    <row r="27" spans="1:12">
+      <c r="A27" s="5">
+        <v>41841</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="15" t="s">
-        <v>47</v>
-      </c>
+      <c r="E27" s="15"/>
       <c r="F27" s="23"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1320,16 +1322,12 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>45</v>
-      </c>
+    <row r="28" spans="1:12">
+      <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="E28" s="15"/>
       <c r="F28" s="23"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1338,7 +1336,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1349,7 +1347,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1360,7 +1358,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1371,7 +1369,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1382,7 +1380,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1393,7 +1391,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1404,7 +1402,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1430,24 +1428,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>